<commit_message>
screen shot for the test result
</commit_message>
<xml_diff>
--- a/Code/Python/VSB_Plus Test/data/case.xlsx
+++ b/Code/Python/VSB_Plus Test/data/case.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="3"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Course search test" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>case number</t>
   </si>
@@ -31,10 +31,7 @@
     <t>Expected Result</t>
   </si>
   <si>
-    <t>case1</t>
-  </si>
-  <si>
-    <t>courseDB_test</t>
+    <t>searchCourse</t>
   </si>
   <si>
     <t>{"short_name": "CHEM 104"}</t>
@@ -43,42 +40,33 @@
     <t>{"suc": "1","assert": "General Chemistry I"}</t>
   </si>
   <si>
-    <t>case2</t>
-  </si>
-  <si>
     <t>{"short_name": "CHEM 103"}</t>
   </si>
   <si>
     <t>{"suc": "0","assert": "CHEM 103 cannot be found"}</t>
   </si>
   <si>
-    <t>case3</t>
-  </si>
-  <si>
     <t>{"short_name": "CS 210"}</t>
   </si>
   <si>
     <t>{"suc": "1","assert": "Data Structures and Abstractions"}</t>
   </si>
   <si>
-    <t>case4</t>
-  </si>
-  <si>
     <t>{"short_name": "CS 215"}</t>
   </si>
   <si>
     <t>{"suc": "1","assert": "Web and Database Programming"}</t>
   </si>
   <si>
-    <t>case5</t>
-  </si>
-  <si>
     <t>{"short_name": "ENEL 487"}</t>
   </si>
   <si>
     <t>{"suc": "1","assert": "Embedded and Real-Time Software Systems"}</t>
   </si>
   <si>
+    <t>faultyFilter</t>
+  </si>
+  <si>
     <t>{"faulty": "ENSE"}</t>
   </si>
   <si>
@@ -160,7 +148,7 @@
     <t>Empty password and sid</t>
   </si>
   <si>
-    <t>semester Builder test</t>
+    <t>prereq</t>
   </si>
   <si>
     <t>{"sid": "200362586", "pwd":"200362586", "course":"math 110"}</t>
@@ -204,9 +192,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -218,6 +206,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -226,30 +250,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -279,9 +289,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -295,6 +304,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -312,12 +329,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -326,37 +344,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -371,187 +359,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,6 +564,56 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,21 +642,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -627,47 +650,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -685,130 +673,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1137,8 +1125,8 @@
   <sheetPr/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="3"/>
@@ -1164,73 +1152,73 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="D6" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1245,7 +1233,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="3"/>
@@ -1271,73 +1259,73 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D6" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1351,8 +1339,8 @@
   <sheetPr/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="4"/>
@@ -1378,92 +1366,92 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>38</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>39</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
         <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1477,8 +1465,8 @@
   <sheetPr/>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -1504,75 +1492,75 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>54</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the drag and drop function and test case
</commit_message>
<xml_diff>
--- a/Code/Python/VSB_Plus Test/data/case.xlsx
+++ b/Code/Python/VSB_Plus Test/data/case.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Course search test" sheetId="1" r:id="rId1"/>
     <sheet name="faulty filter" sheetId="2" r:id="rId2"/>
     <sheet name="Login data" sheetId="3" r:id="rId3"/>
     <sheet name="SemesterBuilder" sheetId="4" r:id="rId4"/>
+    <sheet name="AcademicBuilder" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
   <si>
     <t>case number</t>
   </si>
@@ -185,6 +186,27 @@
   </si>
   <si>
     <t xml:space="preserve">Invaild input course </t>
+  </si>
+  <si>
+    <t>Academic Builder</t>
+  </si>
+  <si>
+    <t>{"sid": "200362878", "pwd":"200362878", "course":"[['MATH 110']]"}</t>
+  </si>
+  <si>
+    <t>{"suc": "1","assert": "3"}</t>
+  </si>
+  <si>
+    <t>Success drag the course</t>
+  </si>
+  <si>
+    <t>{"sid": "200362878", "pwd":"200362878", "course":"[['MATH 111']]"}</t>
+  </si>
+  <si>
+    <t>{"suc": "0","assert": "Prerequisites [Not Matched]:"}</t>
+  </si>
+  <si>
+    <t>Drag the course that prere is not satisfy</t>
   </si>
 </sst>
 </file>
@@ -192,10 +214,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -206,6 +228,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -214,7 +252,99 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,122 +359,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -359,187 +381,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -553,37 +575,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -599,21 +595,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -642,11 +623,52 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -655,7 +677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -673,130 +695,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1339,7 +1361,7 @@
   <sheetPr/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1466,7 +1488,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -1567,4 +1589,79 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="21.4444444444444" customWidth="1"/>
+    <col min="3" max="3" width="59.7777777777778" customWidth="1"/>
+    <col min="4" max="4" width="48" customWidth="1"/>
+    <col min="5" max="5" width="44.5555555555556" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test case / result update
</commit_message>
<xml_diff>
--- a/Code/Python/VSB_Plus Test/data/case.xlsx
+++ b/Code/Python/VSB_Plus Test/data/case.xlsx
@@ -155,7 +155,7 @@
     <t>{"sid": "200362586", "pwd":"200362586", "course":"ENGL 100"}</t>
   </si>
   <si>
-    <t>{"suc": "1","assert": "MATH 110 registration success."}</t>
+    <t>{"suc": "1","assert": "ENGL 100 registration success."}</t>
   </si>
   <si>
     <t>Success add course</t>
@@ -226,10 +226,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -240,8 +240,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,13 +257,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,11 +270,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -286,7 +294,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,11 +339,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -348,29 +370,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -393,187 +393,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,15 +584,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -607,6 +598,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -645,21 +651,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -670,6 +661,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -689,148 +689,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1500,7 +1500,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D6" sqref="D2 D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="4"/>

</xml_diff>